<commit_message>
completed Working with dimentions
</commit_message>
<xml_diff>
--- a/0_Resourse/PL300_resource.xlsx
+++ b/0_Resourse/PL300_resource.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\me\Microsoft\Power bi\0_Resourse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73071E36-FAB8-4C8A-A1D0-F2CE7EABFAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E663953-9DEF-4117-BD03-70F8AB7B4DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E8B07B39-923F-4FFF-916F-9B411939DA27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" r:id="rId1"/>
     <sheet name="Orders" sheetId="2" r:id="rId2"/>
+    <sheet name="Employee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="49">
   <si>
     <t>SalesOrderID</t>
   </si>
@@ -136,12 +137,45 @@
   <si>
     <t>Women</t>
   </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Manager ID</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Roy F</t>
+  </si>
+  <si>
+    <t>Pam H</t>
+  </si>
+  <si>
+    <t>Guy L</t>
+  </si>
+  <si>
+    <t>Roger M</t>
+  </si>
+  <si>
+    <t>Kaylie S</t>
+  </si>
+  <si>
+    <t>Mike O</t>
+  </si>
+  <si>
+    <t>Rudy Q</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +309,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="33">
@@ -458,7 +497,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -573,6 +612,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -618,9 +672,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -976,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF676F34-8B0B-422C-90F1-E00A791FABE6}">
-  <dimension ref="A1:J201"/>
+  <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="K196" sqref="K196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,7 +1044,7 @@
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1018,8 +1075,11 @@
       <c r="J1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1050,8 +1110,11 @@
       <c r="J2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1082,8 +1145,11 @@
       <c r="J3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1114,8 +1180,11 @@
       <c r="J4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1146,8 +1215,11 @@
       <c r="J5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1178,8 +1250,11 @@
       <c r="J6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1210,8 +1285,11 @@
       <c r="J7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1242,8 +1320,11 @@
       <c r="J8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1274,8 +1355,11 @@
       <c r="J9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1306,8 +1390,11 @@
       <c r="J10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1338,8 +1425,11 @@
       <c r="J11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1370,8 +1460,11 @@
       <c r="J12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1402,8 +1495,11 @@
       <c r="J13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1434,8 +1530,11 @@
       <c r="J14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1466,8 +1565,11 @@
       <c r="J15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1498,8 +1600,11 @@
       <c r="J16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1530,8 +1635,11 @@
       <c r="J17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1562,8 +1670,11 @@
       <c r="J18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1594,8 +1705,11 @@
       <c r="J19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1626,8 +1740,11 @@
       <c r="J20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1658,8 +1775,11 @@
       <c r="J21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1690,8 +1810,11 @@
       <c r="J22" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1722,8 +1845,11 @@
       <c r="J23" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1754,8 +1880,11 @@
       <c r="J24" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1786,8 +1915,11 @@
       <c r="J25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1818,8 +1950,11 @@
       <c r="J26" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1850,8 +1985,11 @@
       <c r="J27" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1882,8 +2020,11 @@
       <c r="J28" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1914,8 +2055,11 @@
       <c r="J29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1946,8 +2090,11 @@
       <c r="J30" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1978,8 +2125,11 @@
       <c r="J31" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2010,8 +2160,11 @@
       <c r="J32" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2042,8 +2195,11 @@
       <c r="J33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2074,8 +2230,11 @@
       <c r="J34" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2106,8 +2265,11 @@
       <c r="J35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K35">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2138,8 +2300,11 @@
       <c r="J36" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K36">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2170,8 +2335,11 @@
       <c r="J37" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K37">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2202,8 +2370,11 @@
       <c r="J38" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K38">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2234,8 +2405,11 @@
       <c r="J39" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K39">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2266,8 +2440,11 @@
       <c r="J40" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K40">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2298,8 +2475,11 @@
       <c r="J41" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K41">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2330,8 +2510,11 @@
       <c r="J42" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K42">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2362,8 +2545,11 @@
       <c r="J43" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K43">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2394,8 +2580,11 @@
       <c r="J44" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K44">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2426,8 +2615,11 @@
       <c r="J45" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K45">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2458,8 +2650,11 @@
       <c r="J46" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K46">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2490,8 +2685,11 @@
       <c r="J47" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K47">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2522,8 +2720,11 @@
       <c r="J48" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K48">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2554,8 +2755,11 @@
       <c r="J49" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K49">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2586,8 +2790,11 @@
       <c r="J50" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K50">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2618,8 +2825,11 @@
       <c r="J51" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K51">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2650,8 +2860,11 @@
       <c r="J52" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K52">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2682,8 +2895,11 @@
       <c r="J53" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K53">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2714,8 +2930,11 @@
       <c r="J54" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K54">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2746,8 +2965,11 @@
       <c r="J55" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K55">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2778,8 +3000,11 @@
       <c r="J56" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K56">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2810,8 +3035,11 @@
       <c r="J57" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K57">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2842,8 +3070,11 @@
       <c r="J58" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K58">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2874,8 +3105,11 @@
       <c r="J59" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K59">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2906,8 +3140,11 @@
       <c r="J60" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K60">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2938,8 +3175,11 @@
       <c r="J61" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K61">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2970,8 +3210,11 @@
       <c r="J62" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K62">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3002,8 +3245,11 @@
       <c r="J63" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K63">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3034,8 +3280,11 @@
       <c r="J64" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K64">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3066,8 +3315,11 @@
       <c r="J65" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K65">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3098,8 +3350,11 @@
       <c r="J66" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K66">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3130,8 +3385,11 @@
       <c r="J67" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K67">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3162,8 +3420,11 @@
       <c r="J68" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K68">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3194,8 +3455,11 @@
       <c r="J69" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K69">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3226,8 +3490,11 @@
       <c r="J70" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K70">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3258,8 +3525,11 @@
       <c r="J71" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K71">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3290,8 +3560,11 @@
       <c r="J72" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K72">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3322,8 +3595,11 @@
       <c r="J73" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K73">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3354,8 +3630,11 @@
       <c r="J74" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K74">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3386,8 +3665,11 @@
       <c r="J75" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K75">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3418,8 +3700,11 @@
       <c r="J76" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K76">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3450,8 +3735,11 @@
       <c r="J77" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K77">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3482,8 +3770,11 @@
       <c r="J78" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K78">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3514,8 +3805,11 @@
       <c r="J79" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K79">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3546,8 +3840,11 @@
       <c r="J80" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K80">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3578,8 +3875,11 @@
       <c r="J81" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K81">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3610,8 +3910,11 @@
       <c r="J82" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K82">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3642,8 +3945,11 @@
       <c r="J83" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K83">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3674,8 +3980,11 @@
       <c r="J84" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K84">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3706,8 +4015,11 @@
       <c r="J85" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K85">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3738,8 +4050,11 @@
       <c r="J86" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K86">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3770,8 +4085,11 @@
       <c r="J87" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K87">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3802,8 +4120,11 @@
       <c r="J88" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K88">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3834,8 +4155,11 @@
       <c r="J89" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K89">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3866,8 +4190,11 @@
       <c r="J90" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K90">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3898,8 +4225,11 @@
       <c r="J91" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K91">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3930,8 +4260,11 @@
       <c r="J92" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K92">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3962,8 +4295,11 @@
       <c r="J93" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K93">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3994,8 +4330,11 @@
       <c r="J94" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K94">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4026,8 +4365,11 @@
       <c r="J95" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K95">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4058,8 +4400,11 @@
       <c r="J96" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K96">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4090,8 +4435,11 @@
       <c r="J97" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K97">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4122,8 +4470,11 @@
       <c r="J98" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K98">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4154,8 +4505,11 @@
       <c r="J99" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K99">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4186,8 +4540,11 @@
       <c r="J100" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K100">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4218,8 +4575,11 @@
       <c r="J101" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K101">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4250,8 +4610,11 @@
       <c r="J102" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K102">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4282,8 +4645,11 @@
       <c r="J103" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K103">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4314,8 +4680,11 @@
       <c r="J104" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K104">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4346,8 +4715,11 @@
       <c r="J105" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K105">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4378,8 +4750,11 @@
       <c r="J106" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K106">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4410,8 +4785,11 @@
       <c r="J107" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K107">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4442,8 +4820,11 @@
       <c r="J108" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K108">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4474,8 +4855,11 @@
       <c r="J109" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K109">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4506,8 +4890,11 @@
       <c r="J110" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K110">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4538,8 +4925,11 @@
       <c r="J111" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K111">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4570,8 +4960,11 @@
       <c r="J112" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K112">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4602,8 +4995,11 @@
       <c r="J113" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K113">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4634,8 +5030,11 @@
       <c r="J114" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K114">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4666,8 +5065,11 @@
       <c r="J115" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K115">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4698,8 +5100,11 @@
       <c r="J116" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K116">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4730,8 +5135,11 @@
       <c r="J117" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K117">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4762,8 +5170,11 @@
       <c r="J118" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K118">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4794,8 +5205,11 @@
       <c r="J119" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K119">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4826,8 +5240,11 @@
       <c r="J120" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K120">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4858,8 +5275,11 @@
       <c r="J121" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K121">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4890,8 +5310,11 @@
       <c r="J122" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K122">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4922,8 +5345,11 @@
       <c r="J123" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K123">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4954,8 +5380,11 @@
       <c r="J124" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K124">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4986,8 +5415,11 @@
       <c r="J125" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K125">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5018,8 +5450,11 @@
       <c r="J126" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K126">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5050,8 +5485,11 @@
       <c r="J127" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K127">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5082,8 +5520,11 @@
       <c r="J128" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K128">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5114,8 +5555,11 @@
       <c r="J129" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K129">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5146,8 +5590,11 @@
       <c r="J130" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K130">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5178,8 +5625,11 @@
       <c r="J131" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K131">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5210,8 +5660,11 @@
       <c r="J132" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K132">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5242,8 +5695,11 @@
       <c r="J133" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K133">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5274,8 +5730,11 @@
       <c r="J134" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K134">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5306,8 +5765,11 @@
       <c r="J135" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K135">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5338,8 +5800,11 @@
       <c r="J136" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K136">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5370,8 +5835,11 @@
       <c r="J137" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K137">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5402,8 +5870,11 @@
       <c r="J138" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K138">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5434,8 +5905,11 @@
       <c r="J139" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K139">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5466,8 +5940,11 @@
       <c r="J140" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K140">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5498,8 +5975,11 @@
       <c r="J141" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K141">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5530,8 +6010,11 @@
       <c r="J142" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K142">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5562,8 +6045,11 @@
       <c r="J143" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K143">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5594,8 +6080,11 @@
       <c r="J144" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K144">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5626,8 +6115,11 @@
       <c r="J145" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K145">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5658,8 +6150,11 @@
       <c r="J146" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K146">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5690,8 +6185,11 @@
       <c r="J147" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K147">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5722,8 +6220,11 @@
       <c r="J148" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K148">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5754,8 +6255,11 @@
       <c r="J149" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K149">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5786,8 +6290,11 @@
       <c r="J150" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K150">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5818,8 +6325,11 @@
       <c r="J151" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K151">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5850,8 +6360,11 @@
       <c r="J152" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K152">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5882,8 +6395,11 @@
       <c r="J153" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K153">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5914,8 +6430,11 @@
       <c r="J154" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K154">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>154</v>
       </c>
@@ -5946,8 +6465,11 @@
       <c r="J155" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K155">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>155</v>
       </c>
@@ -5978,8 +6500,11 @@
       <c r="J156" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K156">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>156</v>
       </c>
@@ -6010,8 +6535,11 @@
       <c r="J157" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K157">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>157</v>
       </c>
@@ -6042,8 +6570,11 @@
       <c r="J158" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K158">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>158</v>
       </c>
@@ -6074,8 +6605,11 @@
       <c r="J159" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K159">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>159</v>
       </c>
@@ -6106,8 +6640,11 @@
       <c r="J160" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K160">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6138,8 +6675,11 @@
       <c r="J161" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K161">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6170,8 +6710,11 @@
       <c r="J162" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K162">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
@@ -6202,8 +6745,11 @@
       <c r="J163" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K163">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6234,8 +6780,11 @@
       <c r="J164" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K164">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
@@ -6266,8 +6815,11 @@
       <c r="J165" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K165">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6298,8 +6850,11 @@
       <c r="J166" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K166">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6330,8 +6885,11 @@
       <c r="J167" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K167">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6362,8 +6920,11 @@
       <c r="J168" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K168">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6394,8 +6955,11 @@
       <c r="J169" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K169">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6426,8 +6990,11 @@
       <c r="J170" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K170">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
@@ -6458,8 +7025,11 @@
       <c r="J171" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K171">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
@@ -6490,8 +7060,11 @@
       <c r="J172" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K172">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
@@ -6522,8 +7095,11 @@
       <c r="J173" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K173">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
@@ -6554,8 +7130,11 @@
       <c r="J174" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K174">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
@@ -6586,8 +7165,11 @@
       <c r="J175" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K175">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
@@ -6618,8 +7200,11 @@
       <c r="J176" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K176">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>176</v>
       </c>
@@ -6650,8 +7235,11 @@
       <c r="J177" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K177">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>177</v>
       </c>
@@ -6682,8 +7270,11 @@
       <c r="J178" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K178">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>178</v>
       </c>
@@ -6714,8 +7305,11 @@
       <c r="J179" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K179">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
@@ -6746,8 +7340,11 @@
       <c r="J180" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K180">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
@@ -6778,8 +7375,11 @@
       <c r="J181" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K181">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
@@ -6810,8 +7410,11 @@
       <c r="J182" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K182">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
@@ -6842,8 +7445,11 @@
       <c r="J183" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K183">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
@@ -6874,8 +7480,11 @@
       <c r="J184" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K184">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>184</v>
       </c>
@@ -6906,8 +7515,11 @@
       <c r="J185" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K185">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>185</v>
       </c>
@@ -6938,8 +7550,11 @@
       <c r="J186" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K186">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>186</v>
       </c>
@@ -6970,8 +7585,11 @@
       <c r="J187" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K187">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>187</v>
       </c>
@@ -7002,8 +7620,11 @@
       <c r="J188" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K188">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>188</v>
       </c>
@@ -7034,8 +7655,11 @@
       <c r="J189" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K189">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>189</v>
       </c>
@@ -7066,8 +7690,11 @@
       <c r="J190" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K190">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>190</v>
       </c>
@@ -7098,8 +7725,11 @@
       <c r="J191" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K191">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>191</v>
       </c>
@@ -7130,8 +7760,11 @@
       <c r="J192" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K192">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>192</v>
       </c>
@@ -7162,8 +7795,11 @@
       <c r="J193" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K193">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>193</v>
       </c>
@@ -7194,8 +7830,11 @@
       <c r="J194" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K194">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>194</v>
       </c>
@@ -7226,8 +7865,11 @@
       <c r="J195" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K195">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>195</v>
       </c>
@@ -7258,8 +7900,11 @@
       <c r="J196" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K196">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>196</v>
       </c>
@@ -7290,8 +7935,11 @@
       <c r="J197" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K197">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>197</v>
       </c>
@@ -7322,8 +7970,11 @@
       <c r="J198" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K198">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>198</v>
       </c>
@@ -7354,8 +8005,11 @@
       <c r="J199" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K199">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>199</v>
       </c>
@@ -7386,8 +8040,11 @@
       <c r="J200" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K200">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>200</v>
       </c>
@@ -7417,6 +8074,9 @@
       </c>
       <c r="J201" t="s">
         <v>30</v>
+      </c>
+      <c r="K201">
+        <v>1012</v>
       </c>
     </row>
   </sheetData>
@@ -13272,4 +13932,131 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF8F8C2-F855-478A-A2FB-0CFEC00D4EA8}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1010</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1011</v>
+      </c>
+      <c r="B3">
+        <v>1010</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1012</v>
+      </c>
+      <c r="B4">
+        <v>1010</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1013</v>
+      </c>
+      <c r="B5">
+        <v>1011</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1014</v>
+      </c>
+      <c r="B6">
+        <v>1011</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1015</v>
+      </c>
+      <c r="B7">
+        <v>1012</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1016</v>
+      </c>
+      <c r="B8">
+        <v>1012</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>